<commit_message>
web scrapping dynamic web pages
</commit_message>
<xml_diff>
--- a/quotes.xlsx
+++ b/quotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\Backup\Web Scrapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF59FEC5-622D-495F-B631-7C438EFBA23A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED8AC326-DD4D-4176-B4E7-0228992B702A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="3050" yWindow="1690" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Quote</t>
   </si>
@@ -28,58 +28,46 @@
     <t>Author</t>
   </si>
   <si>
-    <t>“The world as we have created it is a process of our thinking. It cannot be changed without changing our thinking.”</t>
-  </si>
-  <si>
-    <t>Albert Einstein</t>
-  </si>
-  <si>
-    <t>“It is our choices, Harry, that show what we truly are, far more than our abilities.”</t>
-  </si>
-  <si>
-    <t>J.K. Rowling</t>
-  </si>
-  <si>
-    <t>“There are only two ways to live your life. One is as though nothing is a miracle. The other is as though everything is a miracle.”</t>
-  </si>
-  <si>
-    <t>“The person, be it gentleman or lady, who has not pleasure in a good novel, must be intolerably stupid.”</t>
+    <t>“The more that you read, the more things you will know. The more that you learn, the more places you'll go.”</t>
+  </si>
+  <si>
+    <t>Dr. Seuss</t>
+  </si>
+  <si>
+    <t>“We read to know we're not alone.”</t>
+  </si>
+  <si>
+    <t>William Nicholson</t>
+  </si>
+  <si>
+    <t>“A reader lives a thousand lives before he dies, said Jojen. The man who never reads lives only one.”</t>
+  </si>
+  <si>
+    <t>George R.R. Martin</t>
+  </si>
+  <si>
+    <t>“You can never get a cup of tea large enough or a book long enough to suit me.”</t>
+  </si>
+  <si>
+    <t>C.S. Lewis</t>
+  </si>
+  <si>
+    <t>“What really knocks me out is a book that, when you're all done reading it, you wish the author that wrote it was a terrific friend of yours and you could call him up on the phone whenever you felt like it. That doesn't happen much, though.”</t>
+  </si>
+  <si>
+    <t>J.D. Salinger</t>
+  </si>
+  <si>
+    <t>“′Classic′ - a book which people praise and don't read.”</t>
+  </si>
+  <si>
+    <t>Mark Twain</t>
+  </si>
+  <si>
+    <t>“I declare after all there is no enjoyment like reading! How much sooner one tires of any thing than of a book! -- When I have a house of my own, I shall be miserable if I have not an excellent library.”</t>
   </si>
   <si>
     <t>Jane Austen</t>
-  </si>
-  <si>
-    <t>“Imperfection is beauty, madness is genius and it's better to be absolutely ridiculous than absolutely boring.”</t>
-  </si>
-  <si>
-    <t>Marilyn Monroe</t>
-  </si>
-  <si>
-    <t>“Try not to become a man of success. Rather become a man of value.”</t>
-  </si>
-  <si>
-    <t>“It is better to be hated for what you are than to be loved for what you are not.”</t>
-  </si>
-  <si>
-    <t>André Gide</t>
-  </si>
-  <si>
-    <t>“I have not failed. I've just found 10,000 ways that won't work.”</t>
-  </si>
-  <si>
-    <t>Thomas A. Edison</t>
-  </si>
-  <si>
-    <t>“A woman is like a tea bag; you never know how strong it is until it's in hot water.”</t>
-  </si>
-  <si>
-    <t>Eleanor Roosevelt</t>
-  </si>
-  <si>
-    <t>“A day without sunshine is like, you know, night.”</t>
-  </si>
-  <si>
-    <t>Steve Martin</t>
   </si>
 </sst>
 </file>
@@ -138,10 +126,10 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -445,17 +433,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="51.54296875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="23.90625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="34.26953125" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -474,7 +461,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -487,63 +474,39 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="87" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="2" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>